<commit_message>
Export to excel now works but still needs more refactoring , had ad issue where edit was missing an update action now fixed!
</commit_message>
<xml_diff>
--- a/aQord.ASP/Files/ExportToExcel/test.xlsx
+++ b/aQord.ASP/Files/ExportToExcel/test.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <x:si>
     <x:t xml:space="preserve">Arbejdets art: </x:t>
   </x:si>
@@ -116,6 +116,12 @@
   </x:si>
   <x:si>
     <x:t>Sø</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Qu</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve"> </x:t>
@@ -1490,27 +1496,61 @@
       <x:c r="V7" s="12" t="s"/>
     </x:row>
     <x:row r="8" spans="1:28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <x:c r="A8" s="83" t="s"/>
-      <x:c r="B8" s="83" t="s"/>
-      <x:c r="C8" s="79" t="s"/>
-      <x:c r="D8" s="84" t="s"/>
-      <x:c r="E8" s="83" t="s"/>
-      <x:c r="F8" s="83" t="s"/>
-      <x:c r="G8" s="83" t="s"/>
-      <x:c r="H8" s="83" t="s"/>
-      <x:c r="I8" s="83" t="s"/>
-      <x:c r="J8" s="83" t="s"/>
+      <x:c r="A8" s="83" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B8" s="83" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C8" s="79" t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D8" s="84" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E8" s="83" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="F8" s="83" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G8" s="83" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="H8" s="83" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I8" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J8" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="K8" s="85">
         <x:f>SUM(D8:J8)</x:f>
       </x:c>
       <x:c r="L8" s="86" t="s"/>
-      <x:c r="M8" s="83" t="s"/>
-      <x:c r="N8" s="83" t="s"/>
-      <x:c r="O8" s="83" t="s"/>
-      <x:c r="P8" s="83" t="s"/>
-      <x:c r="Q8" s="83" t="s"/>
-      <x:c r="R8" s="83" t="s"/>
-      <x:c r="S8" s="83" t="s"/>
+      <x:c r="M8" s="83" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="N8" s="83" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="O8" s="83" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="P8" s="83" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="Q8" s="83" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="R8" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="S8" s="83" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="T8" s="87">
         <x:f>SUM(M8:S8)</x:f>
       </x:c>
@@ -1543,7 +1583,7 @@
         <x:f>SUM(M9:S9)</x:f>
       </x:c>
       <x:c r="U9" s="88" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="V9" s="88" t="s"/>
     </x:row>
@@ -1573,7 +1613,7 @@
         <x:f>SUM(M10:S10)</x:f>
       </x:c>
       <x:c r="U10" s="88" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="V10" s="88" t="s"/>
     </x:row>
@@ -1799,7 +1839,7 @@
         <x:f>SUM(M18:S18)</x:f>
       </x:c>
       <x:c r="U18" s="88" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="V18" s="88" t="s"/>
     </x:row>
@@ -1829,7 +1869,7 @@
         <x:f>SUM(M19:S19)</x:f>
       </x:c>
       <x:c r="U19" s="88" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="V19" s="88" t="s"/>
     </x:row>
@@ -1907,7 +1947,7 @@
     </x:row>
     <x:row r="23" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <x:c r="D23" s="58" t="s">
-        <x:v>28</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E23" s="98" t="s"/>
       <x:c r="F23" s="98" t="s"/>
@@ -1922,7 +1962,7 @@
         <x:f>SUM(L11:L22)</x:f>
       </x:c>
       <x:c r="M23" s="58" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="N23" s="98" t="s"/>
       <x:c r="O23" s="98" t="s"/>
@@ -1944,7 +1984,7 @@
     <x:row r="25" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <x:row r="26" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <x:c r="A26" s="54" t="s">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="B26" s="54" t="s"/>
       <x:c r="C26" s="54" t="s"/>
@@ -1964,7 +2004,7 @@
     <x:row r="27" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <x:row r="28" spans="1:28" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <x:c r="A28" s="54" t="s">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B28" s="54" t="s"/>
       <x:c r="C28" s="54" t="s"/>
@@ -2991,7 +3031,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A1" s="72" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="O1" s="3" t="s"/>
       <x:c r="P1" s="3" t="s"/>
@@ -3036,7 +3076,7 @@
     </x:row>
     <x:row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <x:c r="A3" s="73" t="s">
-        <x:v>33</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="O3" s="3" t="s"/>
       <x:c r="P3" s="3" t="s"/>
@@ -3082,12 +3122,12 @@
     <x:row r="5" spans="1:26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A5" s="3" t="s"/>
       <x:c r="B5" s="21" t="s">
-        <x:v>34</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G5" s="3" t="s"/>
       <x:c r="H5" s="3" t="s"/>
       <x:c r="I5" s="21" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="N5" s="3" t="s"/>
       <x:c r="O5" s="3" t="s"/>
@@ -3134,12 +3174,12 @@
     <x:row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <x:c r="A7" s="3" t="s"/>
       <x:c r="B7" s="73" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G7" s="3" t="s"/>
       <x:c r="H7" s="3" t="s"/>
       <x:c r="I7" s="73" t="s">
-        <x:v>36</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="N7" s="3" t="s"/>
       <x:c r="O7" s="3" t="s"/>
@@ -3157,7 +3197,7 @@
     </x:row>
     <x:row r="8" spans="1:26" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <x:c r="A8" s="25" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B8" s="26" t="s"/>
       <x:c r="C8" s="28" t="s"/>
@@ -3165,10 +3205,10 @@
       <x:c r="E8" s="28" t="s"/>
       <x:c r="F8" s="29" t="s"/>
       <x:c r="G8" s="25" t="s">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="H8" s="25" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="I8" s="26" t="s"/>
       <x:c r="J8" s="28" t="s"/>
@@ -3176,7 +3216,7 @@
       <x:c r="L8" s="28" t="s"/>
       <x:c r="M8" s="29" t="s"/>
       <x:c r="N8" s="25" t="s">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="O8" s="3" t="s"/>
       <x:c r="P8" s="3" t="s"/>

</xml_diff>